<commit_message>
bug fix, add excel report with color coding
</commit_message>
<xml_diff>
--- a/reports/impact/test_impact_report.xlsx
+++ b/reports/impact/test_impact_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,22 +448,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>get_impact_data</t>
+          <t>search_impact</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>search_impact</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>

</xml_diff>